<commit_message>
Se reactiva la tasa por default solo para inicializar la oferta. Se eliminan las tasas anidaddas en FlexibleConsolidation. Se corrige error que provocaba obtener errores en negativo. Al actualizar la comisión de forma manual (por el asesor), ahora actualiza la tasa y comision en la lista de deudas seleccionadas. Se agrega validación para no editar deudas no consolidables/editables. Se agrega funcionalidad para reestablecer tasa cuando fue editada por el asesor. Se agrega validación para cuando se excede el monto de oferta, la tasa será la que viene por defecto.
</commit_message>
<xml_diff>
--- a/json_cons_flex.xlsx
+++ b/json_cons_flex.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidleon/Documents/Python/Lanzamiento_paga_menos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A39259AD-FDBF-8748-A938-DC584EF51F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -121,8 +115,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,10 +128,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -157,54 +157,73 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -237,79 +256,79 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -330,54 +349,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,7 +405,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -396,7 +414,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -405,7 +423,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -413,10 +431,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -445,7 +463,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -458,13 +476,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -482,260 +499,265 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="3">
         <v>128117</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="3">
         <v>198446</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="3">
         <v>300943</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="3">
         <v>380364</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="3">
         <v>399145</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="3">
         <v>631458</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="3">
         <v>715332</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="3">
         <v>956827</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="3">
         <v>1035508</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="3">
         <v>1088954</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="3">
         <v>1115131</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="3">
         <v>1417865</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+      <c r="A14" s="3">
         <v>1425130</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+      <c r="A15" s="3">
         <v>1518951</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+      <c r="A16" s="3">
         <v>1585602</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="3">
         <v>1621574</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="3">
         <v>1690651</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="3">
         <v>1806791</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="3">
         <v>1835040</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="A21" s="3">
         <v>1875623</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+      <c r="A22" s="3">
         <v>1922352</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+      <c r="A23" s="3">
         <v>1931956</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="3">
         <v>1969444</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="3">
         <v>2038744</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="A26" s="3">
         <v>2040191</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="A27" s="3">
         <v>2122223</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+      <c r="A28" s="3">
         <v>2482120</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="3">
         <v>2492170</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="3">
         <v>2850039</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="3">
         <v>2892166</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>